<commit_message>
Correct error in original spec where "Accession number" in MARC 541 spec should be taken to mean "Acquisition number", i.e. our local spec should have read *acq/*ref
</commit_message>
<xml_diff>
--- a/doc/Field translations (in MARC21 order).xlsx
+++ b/doc/Field translations (in MARC21 order).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12924" uniqueCount="6854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12924" uniqueCount="6855">
   <si>
     <t>al</t>
   </si>
@@ -22394,11 +22394,6 @@
     <t>UkCU-P (Suggested by Rick)</t>
   </si>
   <si>
-    <t>*o, *fund, *kb, *sref, *date, *acc/*ref, *pr
-IF record contains multiple *acq groups of fields =&gt; separate 541 field for each *acq group
-NOTES FROM OLD SPEC MOVED TO COLUMN K</t>
-  </si>
-  <si>
     <t>Translation of title
 UPDATE 19.11.15: Added condition that first indicator should be 0 if there is no 1XX field present in the record (1 otherwise)
 Previous note: "Awaiting confirmation this is not repeatable. (Otherwise 242 will need to be turned into a unified macro because otherwise mismatching counts will occur)." dealt with by multipletoptt report, cleared on on 4/4/2016</t>
@@ -22411,6 +22406,14 @@
   </si>
   <si>
     <t>Unclear spec issues need clearing up; should not be too hard. See e-mail 22/3 [Now: Wed, 11 May 2016]</t>
+  </si>
+  <si>
+    <t>*o, *fund, *kb, *sref, *date, *acq/*ref, *pr
+IF record contains multiple *acq groups of fields =&gt; separate 541 field for each *acq group
+NOTES FROM OLD SPEC MOVED TO COLUMN K</t>
+  </si>
+  <si>
+    <t>Accession [Acquisition] number</t>
   </si>
 </sst>
 </file>
@@ -22981,7 +22984,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="426">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -23911,70 +23914,43 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -23983,43 +23959,37 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24029,6 +23999,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24058,40 +24031,91 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24118,26 +24142,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -30634,8 +30640,8 @@
   <dimension ref="A1:K246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -30687,10 +30693,10 @@
     </row>
     <row r="2" spans="1:11" ht="45.75">
       <c r="A2" s="215"/>
-      <c r="B2" s="400" t="s">
+      <c r="B2" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C2" s="401"/>
+      <c r="C2" s="359"/>
       <c r="D2" s="122" t="s">
         <v>299</v>
       </c>
@@ -30708,10 +30714,10 @@
     </row>
     <row r="3" spans="1:11" ht="30.75">
       <c r="A3" s="215"/>
-      <c r="B3" s="398" t="s">
+      <c r="B3" s="366" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="399"/>
+      <c r="C3" s="367"/>
       <c r="D3" s="121" t="s">
         <v>294</v>
       </c>
@@ -30731,10 +30737,10 @@
     </row>
     <row r="4" spans="1:11" ht="214.5">
       <c r="A4" s="214"/>
-      <c r="B4" s="400" t="s">
+      <c r="B4" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C4" s="401"/>
+      <c r="C4" s="359"/>
       <c r="D4" s="122" t="s">
         <v>295</v>
       </c>
@@ -30754,10 +30760,10 @@
     </row>
     <row r="5" spans="1:11" ht="46.5">
       <c r="A5" s="214"/>
-      <c r="B5" s="400" t="s">
+      <c r="B5" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C5" s="401"/>
+      <c r="C5" s="359"/>
       <c r="D5" s="122" t="s">
         <v>296</v>
       </c>
@@ -30777,10 +30783,10 @@
     </row>
     <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="214"/>
-      <c r="B6" s="400" t="s">
+      <c r="B6" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C6" s="401"/>
+      <c r="C6" s="359"/>
       <c r="D6" s="122" t="s">
         <v>303</v>
       </c>
@@ -30800,10 +30806,10 @@
     </row>
     <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="214"/>
-      <c r="B7" s="400" t="s">
+      <c r="B7" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C7" s="401"/>
+      <c r="C7" s="359"/>
       <c r="D7" s="122" t="s">
         <v>306</v>
       </c>
@@ -30823,10 +30829,10 @@
     </row>
     <row r="8" spans="1:11" ht="30.75">
       <c r="A8" s="214"/>
-      <c r="B8" s="400" t="s">
+      <c r="B8" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C8" s="401"/>
+      <c r="C8" s="359"/>
       <c r="D8" s="122" t="s">
         <v>308</v>
       </c>
@@ -30846,10 +30852,10 @@
     </row>
     <row r="9" spans="1:11" ht="30.75">
       <c r="A9" s="214"/>
-      <c r="B9" s="400" t="s">
+      <c r="B9" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C9" s="401"/>
+      <c r="C9" s="359"/>
       <c r="D9" s="122" t="s">
         <v>311</v>
       </c>
@@ -30869,10 +30875,10 @@
     </row>
     <row r="10" spans="1:11" ht="165.75">
       <c r="A10" s="214"/>
-      <c r="B10" s="400" t="s">
+      <c r="B10" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C10" s="401"/>
+      <c r="C10" s="359"/>
       <c r="D10" s="122" t="s">
         <v>313</v>
       </c>
@@ -30890,10 +30896,10 @@
     </row>
     <row r="11" spans="1:11" ht="30.75">
       <c r="A11" s="214"/>
-      <c r="B11" s="400" t="s">
+      <c r="B11" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C11" s="401"/>
+      <c r="C11" s="359"/>
       <c r="D11" s="122" t="s">
         <v>314</v>
       </c>
@@ -30913,10 +30919,10 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="214"/>
-      <c r="B12" s="400" t="s">
+      <c r="B12" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C12" s="401"/>
+      <c r="C12" s="359"/>
       <c r="D12" s="122" t="s">
         <v>297</v>
       </c>
@@ -30936,10 +30942,10 @@
     </row>
     <row r="13" spans="1:11" ht="30.75">
       <c r="A13" s="214"/>
-      <c r="B13" s="400" t="s">
+      <c r="B13" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C13" s="401"/>
+      <c r="C13" s="359"/>
       <c r="D13" s="122" t="s">
         <v>317</v>
       </c>
@@ -30959,10 +30965,10 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="A14" s="214"/>
-      <c r="B14" s="400" t="s">
+      <c r="B14" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C14" s="401"/>
+      <c r="C14" s="359"/>
       <c r="D14" s="122" t="s">
         <v>320</v>
       </c>
@@ -30982,10 +30988,10 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="214"/>
-      <c r="B15" s="400" t="s">
+      <c r="B15" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C15" s="401"/>
+      <c r="C15" s="359"/>
       <c r="D15" s="122" t="s">
         <v>324</v>
       </c>
@@ -31005,10 +31011,10 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16" s="214"/>
-      <c r="B16" s="400" t="s">
+      <c r="B16" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C16" s="401"/>
+      <c r="C16" s="359"/>
       <c r="D16" s="122" t="s">
         <v>326</v>
       </c>
@@ -31028,10 +31034,10 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="214"/>
-      <c r="B17" s="400" t="s">
+      <c r="B17" s="358" t="s">
         <v>293</v>
       </c>
-      <c r="C17" s="401"/>
+      <c r="C17" s="359"/>
       <c r="D17" s="122" t="s">
         <v>329</v>
       </c>
@@ -31765,7 +31771,7 @@
       <c r="H51" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I51" s="380" t="s">
+      <c r="I51" s="360" t="s">
         <v>100</v>
       </c>
       <c r="J51" s="90"/>
@@ -31794,11 +31800,11 @@
       <c r="H52" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="I52" s="351"/>
-      <c r="J52" s="351" t="s">
+      <c r="I52" s="361"/>
+      <c r="J52" s="361" t="s">
         <v>481</v>
       </c>
-      <c r="K52" s="351"/>
+      <c r="K52" s="361"/>
     </row>
     <row r="53" spans="1:11" ht="30">
       <c r="A53" s="230"/>
@@ -31823,9 +31829,9 @@
       <c r="H53" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="I53" s="351"/>
-      <c r="J53" s="351"/>
-      <c r="K53" s="351"/>
+      <c r="I53" s="361"/>
+      <c r="J53" s="361"/>
+      <c r="K53" s="361"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="221"/>
@@ -31863,7 +31869,7 @@
       <c r="H55" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I55" s="357" t="s">
+      <c r="I55" s="364" t="s">
         <v>63</v>
       </c>
       <c r="J55" s="20"/>
@@ -31892,7 +31898,7 @@
       <c r="H56" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I56" s="359"/>
+      <c r="I56" s="365"/>
       <c r="J56" s="25"/>
       <c r="K56" s="24"/>
     </row>
@@ -31930,7 +31936,7 @@
       <c r="H58" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="I58" s="357" t="s">
+      <c r="I58" s="364" t="s">
         <v>493</v>
       </c>
       <c r="J58" s="50"/>
@@ -31959,7 +31965,7 @@
       <c r="H59" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I59" s="358"/>
+      <c r="I59" s="369"/>
       <c r="J59" s="53"/>
       <c r="K59" s="53"/>
     </row>
@@ -31986,7 +31992,7 @@
       <c r="H60" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I60" s="361"/>
+      <c r="I60" s="374"/>
       <c r="J60" s="53"/>
       <c r="K60" s="53"/>
     </row>
@@ -32013,7 +32019,7 @@
       <c r="H61" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="I61" s="362"/>
+      <c r="I61" s="373"/>
       <c r="J61" s="53"/>
       <c r="K61" s="53"/>
     </row>
@@ -32051,10 +32057,10 @@
         <v>496</v>
       </c>
       <c r="H63" s="118"/>
-      <c r="I63" s="380" t="s">
+      <c r="I63" s="360" t="s">
         <v>503</v>
       </c>
-      <c r="J63" s="363" t="s">
+      <c r="J63" s="378" t="s">
         <v>495</v>
       </c>
       <c r="K63" s="118"/>
@@ -32082,8 +32088,8 @@
       <c r="H64" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="I64" s="351"/>
-      <c r="J64" s="382"/>
+      <c r="I64" s="361"/>
+      <c r="J64" s="396"/>
       <c r="K64" s="127"/>
     </row>
     <row r="65" spans="1:11" ht="180">
@@ -32109,8 +32115,8 @@
       <c r="H65" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="I65" s="381"/>
-      <c r="J65" s="383"/>
+      <c r="I65" s="395"/>
+      <c r="J65" s="397"/>
       <c r="K65" s="133"/>
     </row>
     <row r="66" spans="1:11">
@@ -32147,7 +32153,7 @@
       <c r="H67" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="I67" s="380" t="s">
+      <c r="I67" s="360" t="s">
         <v>6239</v>
       </c>
       <c r="J67" s="50"/>
@@ -32176,7 +32182,7 @@
       <c r="H68" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="I68" s="351"/>
+      <c r="I68" s="361"/>
       <c r="J68" s="127"/>
       <c r="K68" s="127"/>
     </row>
@@ -32216,10 +32222,10 @@
       <c r="H70" s="185" t="s">
         <v>26</v>
       </c>
-      <c r="I70" s="373" t="s">
+      <c r="I70" s="389" t="s">
         <v>6776</v>
       </c>
-      <c r="J70" s="364"/>
+      <c r="J70" s="398"/>
       <c r="K70" s="185"/>
     </row>
     <row r="71" spans="1:11">
@@ -32243,8 +32249,8 @@
         <v>69</v>
       </c>
       <c r="H71" s="112"/>
-      <c r="I71" s="374"/>
-      <c r="J71" s="365"/>
+      <c r="I71" s="390"/>
+      <c r="J71" s="372"/>
       <c r="K71" s="116"/>
     </row>
     <row r="72" spans="1:11" ht="45">
@@ -32268,8 +32274,8 @@
         <v>6614</v>
       </c>
       <c r="H72" s="112"/>
-      <c r="I72" s="374"/>
-      <c r="J72" s="365"/>
+      <c r="I72" s="390"/>
+      <c r="J72" s="372"/>
       <c r="K72" s="116"/>
     </row>
     <row r="73" spans="1:11">
@@ -32293,8 +32299,8 @@
         <v>71</v>
       </c>
       <c r="H73" s="160"/>
-      <c r="I73" s="374"/>
-      <c r="J73" s="365"/>
+      <c r="I73" s="390"/>
+      <c r="J73" s="372"/>
       <c r="K73" s="161"/>
     </row>
     <row r="74" spans="1:11">
@@ -32318,8 +32324,8 @@
         <v>73</v>
       </c>
       <c r="H74" s="160"/>
-      <c r="I74" s="374"/>
-      <c r="J74" s="365"/>
+      <c r="I74" s="390"/>
+      <c r="J74" s="372"/>
       <c r="K74" s="161"/>
     </row>
     <row r="75" spans="1:11" ht="75">
@@ -32343,8 +32349,8 @@
         <v>21</v>
       </c>
       <c r="H75" s="160"/>
-      <c r="I75" s="374"/>
-      <c r="J75" s="365"/>
+      <c r="I75" s="390"/>
+      <c r="J75" s="372"/>
       <c r="K75" s="161"/>
     </row>
     <row r="76" spans="1:11" ht="30">
@@ -32368,8 +32374,8 @@
         <v>75</v>
       </c>
       <c r="H76" s="112"/>
-      <c r="I76" s="374"/>
-      <c r="J76" s="365"/>
+      <c r="I76" s="390"/>
+      <c r="J76" s="372"/>
       <c r="K76" s="116"/>
     </row>
     <row r="77" spans="1:11">
@@ -32393,8 +32399,8 @@
         <v>77</v>
       </c>
       <c r="H77" s="112"/>
-      <c r="I77" s="375"/>
-      <c r="J77" s="365"/>
+      <c r="I77" s="391"/>
+      <c r="J77" s="372"/>
       <c r="K77" s="116"/>
     </row>
     <row r="78" spans="1:11">
@@ -32433,10 +32439,10 @@
       <c r="H79" s="185" t="s">
         <v>26</v>
       </c>
-      <c r="I79" s="367" t="s">
+      <c r="I79" s="370" t="s">
         <v>97</v>
       </c>
-      <c r="J79" s="364"/>
+      <c r="J79" s="398"/>
       <c r="K79" s="185"/>
     </row>
     <row r="80" spans="1:11" ht="30">
@@ -32462,8 +32468,8 @@
       <c r="H80" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I80" s="376"/>
-      <c r="J80" s="365"/>
+      <c r="I80" s="388"/>
+      <c r="J80" s="372"/>
       <c r="K80" s="112"/>
     </row>
     <row r="81" spans="1:11">
@@ -32489,8 +32495,8 @@
       <c r="H81" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="I81" s="376"/>
-      <c r="J81" s="365"/>
+      <c r="I81" s="388"/>
+      <c r="J81" s="372"/>
       <c r="K81" s="195"/>
     </row>
     <row r="82" spans="1:11">
@@ -32516,8 +32522,8 @@
       <c r="H82" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="I82" s="377"/>
-      <c r="J82" s="366"/>
+      <c r="I82" s="392"/>
+      <c r="J82" s="399"/>
       <c r="K82" s="136"/>
     </row>
     <row r="83" spans="1:11" ht="15.75">
@@ -32556,10 +32562,10 @@
       <c r="H84" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="I84" s="384" t="s">
+      <c r="I84" s="400" t="s">
         <v>6257</v>
       </c>
-      <c r="J84" s="349"/>
+      <c r="J84" s="401"/>
       <c r="K84" s="110"/>
     </row>
     <row r="85" spans="1:11" ht="30">
@@ -32585,8 +32591,8 @@
       <c r="H85" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I85" s="349"/>
-      <c r="J85" s="350"/>
+      <c r="I85" s="401"/>
+      <c r="J85" s="405"/>
       <c r="K85" s="112"/>
     </row>
     <row r="86" spans="1:11" ht="30">
@@ -32612,8 +32618,8 @@
       <c r="H86" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I86" s="349"/>
-      <c r="J86" s="350"/>
+      <c r="I86" s="401"/>
+      <c r="J86" s="405"/>
       <c r="K86" s="116"/>
     </row>
     <row r="87" spans="1:11" ht="30">
@@ -32639,8 +32645,8 @@
       <c r="H87" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I87" s="349"/>
-      <c r="J87" s="350"/>
+      <c r="I87" s="401"/>
+      <c r="J87" s="405"/>
       <c r="K87" s="112"/>
     </row>
     <row r="88" spans="1:11" ht="48.75" customHeight="1">
@@ -32666,8 +32672,8 @@
       <c r="H88" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I88" s="351"/>
-      <c r="J88" s="351"/>
+      <c r="I88" s="361"/>
+      <c r="J88" s="361"/>
       <c r="K88" s="116"/>
     </row>
     <row r="89" spans="1:11">
@@ -32693,8 +32699,8 @@
       <c r="H89" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="I89" s="351"/>
-      <c r="J89" s="351"/>
+      <c r="I89" s="361"/>
+      <c r="J89" s="361"/>
       <c r="K89" s="112"/>
     </row>
     <row r="90" spans="1:11">
@@ -32733,14 +32739,14 @@
       <c r="H91" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I91" s="357" t="s">
+      <c r="I91" s="364" t="s">
         <v>6767</v>
       </c>
       <c r="J91" s="50"/>
       <c r="K91" s="50"/>
     </row>
     <row r="92" spans="1:11" ht="60">
-      <c r="A92" s="424" t="s">
+      <c r="A92" s="354" t="s">
         <v>6818</v>
       </c>
       <c r="B92" s="52">
@@ -32764,7 +32770,7 @@
       <c r="H92" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I92" s="359"/>
+      <c r="I92" s="365"/>
       <c r="J92" s="53"/>
       <c r="K92" s="53"/>
     </row>
@@ -32799,12 +32805,12 @@
         <v>6838</v>
       </c>
       <c r="G94" s="12" t="s">
-        <v>6851</v>
+        <v>6850</v>
       </c>
       <c r="H94" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I94" s="357" t="s">
+      <c r="I94" s="364" t="s">
         <v>98</v>
       </c>
       <c r="J94" s="20"/>
@@ -32833,7 +32839,7 @@
       <c r="H95" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I95" s="378"/>
+      <c r="I95" s="393"/>
       <c r="J95" s="33"/>
       <c r="K95" s="31"/>
     </row>
@@ -32860,7 +32866,7 @@
       <c r="H96" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I96" s="378"/>
+      <c r="I96" s="393"/>
       <c r="J96" s="33"/>
       <c r="K96" s="31"/>
     </row>
@@ -32887,7 +32893,7 @@
       <c r="H97" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="I97" s="379"/>
+      <c r="I97" s="394"/>
       <c r="J97" s="138"/>
       <c r="K97" s="136"/>
     </row>
@@ -32925,10 +32931,10 @@
         <v>6828</v>
       </c>
       <c r="H99" s="185"/>
-      <c r="I99" s="367" t="s">
+      <c r="I99" s="370" t="s">
         <v>6803</v>
       </c>
-      <c r="J99" s="364"/>
+      <c r="J99" s="398"/>
       <c r="K99" s="185"/>
     </row>
     <row r="100" spans="1:11" ht="30">
@@ -32954,8 +32960,8 @@
       <c r="H100" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="I100" s="365"/>
-      <c r="J100" s="365"/>
+      <c r="I100" s="372"/>
+      <c r="J100" s="372"/>
       <c r="K100" s="208"/>
     </row>
     <row r="101" spans="1:11">
@@ -32981,8 +32987,8 @@
       <c r="H101" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="I101" s="365"/>
-      <c r="J101" s="365"/>
+      <c r="I101" s="372"/>
+      <c r="J101" s="372"/>
       <c r="K101" s="208"/>
     </row>
     <row r="102" spans="1:11" ht="45.75" customHeight="1">
@@ -33008,25 +33014,25 @@
       <c r="H102" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="I102" s="365"/>
-      <c r="J102" s="365"/>
+      <c r="I102" s="372"/>
+      <c r="J102" s="372"/>
       <c r="K102" s="208"/>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="249"/>
-      <c r="B103" s="402" t="s">
+      <c r="B103" s="355" t="s">
         <v>494</v>
       </c>
-      <c r="C103" s="402" t="s">
+      <c r="C103" s="355" t="s">
         <v>57</v>
       </c>
-      <c r="D103" s="368" t="s">
+      <c r="D103" s="402" t="s">
         <v>49</v>
       </c>
-      <c r="E103" s="368" t="s">
+      <c r="E103" s="402" t="s">
         <v>60</v>
       </c>
-      <c r="F103" s="368" t="s">
+      <c r="F103" s="402" t="s">
         <v>6655</v>
       </c>
       <c r="G103" s="208" t="s">
@@ -33035,53 +33041,53 @@
       <c r="H103" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="I103" s="365"/>
-      <c r="J103" s="365"/>
+      <c r="I103" s="372"/>
+      <c r="J103" s="372"/>
       <c r="K103" s="208"/>
     </row>
     <row r="104" spans="1:11" ht="30">
       <c r="A104" s="249"/>
-      <c r="B104" s="403"/>
-      <c r="C104" s="403"/>
-      <c r="D104" s="365"/>
-      <c r="E104" s="365"/>
-      <c r="F104" s="365"/>
+      <c r="B104" s="356"/>
+      <c r="C104" s="356"/>
+      <c r="D104" s="372"/>
+      <c r="E104" s="372"/>
+      <c r="F104" s="372"/>
       <c r="G104" s="208" t="s">
         <v>6653</v>
       </c>
       <c r="H104" s="208"/>
-      <c r="I104" s="365"/>
-      <c r="J104" s="365"/>
+      <c r="I104" s="372"/>
+      <c r="J104" s="372"/>
       <c r="K104" s="208"/>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="249"/>
-      <c r="B105" s="403"/>
-      <c r="C105" s="403"/>
-      <c r="D105" s="365"/>
-      <c r="E105" s="365"/>
-      <c r="F105" s="365"/>
+      <c r="B105" s="356"/>
+      <c r="C105" s="356"/>
+      <c r="D105" s="372"/>
+      <c r="E105" s="372"/>
+      <c r="F105" s="372"/>
       <c r="G105" s="208" t="s">
         <v>6654</v>
       </c>
       <c r="H105" s="208"/>
-      <c r="I105" s="365"/>
-      <c r="J105" s="365"/>
+      <c r="I105" s="372"/>
+      <c r="J105" s="372"/>
       <c r="K105" s="208"/>
     </row>
     <row r="106" spans="1:11" ht="30">
       <c r="A106" s="249"/>
-      <c r="B106" s="404"/>
-      <c r="C106" s="404"/>
-      <c r="D106" s="366"/>
-      <c r="E106" s="366"/>
-      <c r="F106" s="366"/>
+      <c r="B106" s="357"/>
+      <c r="C106" s="357"/>
+      <c r="D106" s="399"/>
+      <c r="E106" s="399"/>
+      <c r="F106" s="399"/>
       <c r="G106" s="136" t="s">
         <v>6657</v>
       </c>
       <c r="H106" s="136"/>
-      <c r="I106" s="365"/>
-      <c r="J106" s="366"/>
+      <c r="I106" s="372"/>
+      <c r="J106" s="399"/>
       <c r="K106" s="136"/>
     </row>
     <row r="107" spans="1:11">
@@ -33118,7 +33124,7 @@
         <v>6223</v>
       </c>
       <c r="H108" s="26"/>
-      <c r="I108" s="357" t="s">
+      <c r="I108" s="364" t="s">
         <v>120</v>
       </c>
       <c r="J108" s="29"/>
@@ -33147,7 +33153,7 @@
       <c r="H109" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I109" s="358"/>
+      <c r="I109" s="369"/>
       <c r="J109" s="33"/>
       <c r="K109" s="31"/>
     </row>
@@ -33174,7 +33180,7 @@
       <c r="H110" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I110" s="358"/>
+      <c r="I110" s="369"/>
       <c r="J110" s="33"/>
       <c r="K110" s="31"/>
     </row>
@@ -33201,7 +33207,7 @@
       <c r="H111" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I111" s="359"/>
+      <c r="I111" s="365"/>
       <c r="J111" s="40"/>
       <c r="K111" s="18"/>
     </row>
@@ -33241,7 +33247,7 @@
       <c r="H113" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I113" s="369" t="s">
+      <c r="I113" s="403" t="s">
         <v>136</v>
       </c>
       <c r="J113" s="16"/>
@@ -33270,7 +33276,7 @@
       <c r="H114" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I114" s="370"/>
+      <c r="I114" s="404"/>
       <c r="J114" s="45"/>
       <c r="K114" s="44"/>
     </row>
@@ -33297,7 +33303,7 @@
       <c r="H115" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I115" s="370"/>
+      <c r="I115" s="404"/>
       <c r="J115" s="17"/>
       <c r="K115" s="36"/>
     </row>
@@ -33337,10 +33343,10 @@
       <c r="H117" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="I117" s="357" t="s">
+      <c r="I117" s="364" t="s">
         <v>137</v>
       </c>
-      <c r="J117" s="357" t="s">
+      <c r="J117" s="364" t="s">
         <v>505</v>
       </c>
       <c r="K117" s="106"/>
@@ -33368,8 +33374,8 @@
       <c r="H118" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="I118" s="358"/>
-      <c r="J118" s="361"/>
+      <c r="I118" s="369"/>
+      <c r="J118" s="374"/>
       <c r="K118" s="127"/>
     </row>
     <row r="119" spans="1:11" ht="45">
@@ -33395,8 +33401,8 @@
       <c r="H119" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="I119" s="358"/>
-      <c r="J119" s="361"/>
+      <c r="I119" s="369"/>
+      <c r="J119" s="374"/>
       <c r="K119" s="127"/>
     </row>
     <row r="120" spans="1:11">
@@ -33422,8 +33428,8 @@
       <c r="H120" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I120" s="359"/>
-      <c r="J120" s="362"/>
+      <c r="I120" s="365"/>
+      <c r="J120" s="373"/>
       <c r="K120" s="24"/>
     </row>
     <row r="121" spans="1:11">
@@ -33462,7 +33468,7 @@
       <c r="H122" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I122" s="357" t="s">
+      <c r="I122" s="364" t="s">
         <v>6247</v>
       </c>
       <c r="J122" s="20"/>
@@ -33491,8 +33497,8 @@
       <c r="H123" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I123" s="358"/>
-      <c r="J123" s="363" t="s">
+      <c r="I123" s="369"/>
+      <c r="J123" s="378" t="s">
         <v>139</v>
       </c>
       <c r="K123" s="19"/>
@@ -33520,8 +33526,8 @@
       <c r="H124" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I124" s="358"/>
-      <c r="J124" s="359"/>
+      <c r="I124" s="369"/>
+      <c r="J124" s="365"/>
       <c r="K124" s="31"/>
     </row>
     <row r="125" spans="1:11">
@@ -33547,7 +33553,7 @@
       <c r="H125" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I125" s="358"/>
+      <c r="I125" s="369"/>
       <c r="J125" s="54"/>
       <c r="K125" s="53"/>
     </row>
@@ -33574,7 +33580,7 @@
       <c r="H126" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I126" s="359"/>
+      <c r="I126" s="365"/>
       <c r="J126" s="40" t="s">
         <v>139</v>
       </c>
@@ -33616,7 +33622,7 @@
       <c r="H128" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I128" s="357" t="s">
+      <c r="I128" s="364" t="s">
         <v>149</v>
       </c>
       <c r="J128" s="20"/>
@@ -33645,7 +33651,7 @@
       <c r="H129" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I129" s="359"/>
+      <c r="I129" s="365"/>
       <c r="J129" s="58"/>
       <c r="K129" s="56"/>
     </row>
@@ -33685,7 +33691,7 @@
       <c r="H131" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="I131" s="357" t="s">
+      <c r="I131" s="364" t="s">
         <v>155</v>
       </c>
       <c r="J131" s="171"/>
@@ -33714,7 +33720,7 @@
       <c r="H132" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I132" s="358"/>
+      <c r="I132" s="369"/>
       <c r="J132" s="33"/>
       <c r="K132" s="31"/>
     </row>
@@ -33741,7 +33747,7 @@
       <c r="H133" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I133" s="359"/>
+      <c r="I133" s="365"/>
       <c r="J133" s="40"/>
       <c r="K133" s="36"/>
     </row>
@@ -33781,7 +33787,7 @@
       <c r="H135" s="305" t="s">
         <v>26</v>
       </c>
-      <c r="I135" s="371" t="s">
+      <c r="I135" s="362" t="s">
         <v>159</v>
       </c>
       <c r="J135" s="306"/>
@@ -33810,7 +33816,7 @@
       <c r="H136" s="310" t="s">
         <v>26</v>
       </c>
-      <c r="I136" s="372"/>
+      <c r="I136" s="363"/>
       <c r="J136" s="311"/>
       <c r="K136" s="309"/>
     </row>
@@ -33850,7 +33856,7 @@
       <c r="H138" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I138" s="357" t="s">
+      <c r="I138" s="364" t="s">
         <v>163</v>
       </c>
       <c r="J138" s="20"/>
@@ -33879,7 +33885,7 @@
       <c r="H139" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I139" s="359"/>
+      <c r="I139" s="365"/>
       <c r="J139" s="58"/>
       <c r="K139" s="56"/>
     </row>
@@ -33897,8 +33903,8 @@
       <c r="K140" s="9"/>
     </row>
     <row r="141" spans="1:11" ht="189">
-      <c r="A141" s="423" t="s">
-        <v>6853</v>
+      <c r="A141" s="353" t="s">
+        <v>6852</v>
       </c>
       <c r="B141" s="73">
         <v>0</v>
@@ -33912,14 +33918,14 @@
       <c r="E141" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="F141" s="345" t="s">
-        <v>6850</v>
+      <c r="F141" s="349" t="s">
+        <v>6853</v>
       </c>
       <c r="G141" s="345" t="s">
         <v>197</v>
       </c>
       <c r="H141" s="75"/>
-      <c r="I141" s="357" t="s">
+      <c r="I141" s="364" t="s">
         <v>512</v>
       </c>
       <c r="J141" s="15"/>
@@ -33948,7 +33954,7 @@
       <c r="H142" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I142" s="360"/>
+      <c r="I142" s="368"/>
       <c r="J142" s="15"/>
       <c r="K142" s="226" t="s">
         <v>6809</v>
@@ -33977,7 +33983,7 @@
       <c r="H143" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I143" s="358"/>
+      <c r="I143" s="369"/>
       <c r="J143" s="54" t="s">
         <v>6241</v>
       </c>
@@ -34008,7 +34014,7 @@
       <c r="H144" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I144" s="361"/>
+      <c r="I144" s="374"/>
       <c r="J144" s="54" t="s">
         <v>204</v>
       </c>
@@ -34031,15 +34037,15 @@
         <v>60</v>
       </c>
       <c r="F145" s="51" t="s">
-        <v>67</v>
+        <v>194</v>
       </c>
       <c r="G145" s="51" t="s">
-        <v>20</v>
+        <v>6854</v>
       </c>
       <c r="H145" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I145" s="361"/>
+      <c r="I145" s="374"/>
       <c r="J145" s="54" t="s">
         <v>206</v>
       </c>
@@ -34070,7 +34076,7 @@
       <c r="H146" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I146" s="362"/>
+      <c r="I146" s="373"/>
       <c r="J146" s="54" t="s">
         <v>210</v>
       </c>
@@ -34133,7 +34139,7 @@
       <c r="H149" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I149" s="357" t="s">
+      <c r="I149" s="364" t="s">
         <v>167</v>
       </c>
       <c r="J149" s="20"/>
@@ -34162,7 +34168,7 @@
       <c r="H150" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="I150" s="359"/>
+      <c r="I150" s="365"/>
       <c r="J150" s="58"/>
       <c r="K150" s="56"/>
     </row>
@@ -34202,7 +34208,7 @@
       <c r="H152" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I152" s="357" t="s">
+      <c r="I152" s="364" t="s">
         <v>171</v>
       </c>
       <c r="J152" s="20"/>
@@ -34231,7 +34237,7 @@
       <c r="H153" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="I153" s="359"/>
+      <c r="I153" s="365"/>
       <c r="J153" s="58"/>
       <c r="K153" s="56"/>
     </row>
@@ -34290,10 +34296,10 @@
       <c r="H156" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I156" s="380" t="s">
+      <c r="I156" s="360" t="s">
         <v>6784</v>
       </c>
-      <c r="J156" s="356" t="s">
+      <c r="J156" s="410" t="s">
         <v>510</v>
       </c>
       <c r="K156" s="50"/>
@@ -34321,8 +34327,8 @@
       <c r="H157" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I157" s="380"/>
-      <c r="J157" s="356"/>
+      <c r="I157" s="360"/>
+      <c r="J157" s="410"/>
       <c r="K157" s="50"/>
     </row>
     <row r="158" spans="1:11" ht="315">
@@ -34348,8 +34354,8 @@
       <c r="H158" s="266" t="s">
         <v>26</v>
       </c>
-      <c r="I158" s="351"/>
-      <c r="J158" s="356"/>
+      <c r="I158" s="361"/>
+      <c r="J158" s="410"/>
       <c r="K158" s="266"/>
     </row>
     <row r="159" spans="1:11">
@@ -34388,10 +34394,10 @@
       <c r="H160" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I160" s="357" t="s">
+      <c r="I160" s="364" t="s">
         <v>6777</v>
       </c>
-      <c r="J160" s="390" t="s">
+      <c r="J160" s="380" t="s">
         <v>511</v>
       </c>
       <c r="K160" s="21"/>
@@ -34419,8 +34425,8 @@
       <c r="H161" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="I161" s="360"/>
-      <c r="J161" s="391"/>
+      <c r="I161" s="368"/>
+      <c r="J161" s="381"/>
       <c r="K161" s="21"/>
     </row>
     <row r="162" spans="1:11" ht="180">
@@ -34446,8 +34452,8 @@
       <c r="H162" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="I162" s="358"/>
-      <c r="J162" s="391"/>
+      <c r="I162" s="369"/>
+      <c r="J162" s="381"/>
       <c r="K162" s="129"/>
     </row>
     <row r="163" spans="1:11">
@@ -34486,7 +34492,7 @@
       <c r="H164" s="189" t="s">
         <v>26</v>
       </c>
-      <c r="I164" s="352" t="s">
+      <c r="I164" s="406" t="s">
         <v>6773</v>
       </c>
       <c r="J164" s="158" t="s">
@@ -34517,8 +34523,8 @@
       <c r="H165" s="190" t="s">
         <v>26</v>
       </c>
-      <c r="I165" s="353"/>
-      <c r="J165" s="357" t="s">
+      <c r="I165" s="407"/>
+      <c r="J165" s="364" t="s">
         <v>47</v>
       </c>
       <c r="K165" s="127"/>
@@ -34544,8 +34550,8 @@
         <v>6614</v>
       </c>
       <c r="H166" s="112"/>
-      <c r="I166" s="353"/>
-      <c r="J166" s="360"/>
+      <c r="I166" s="407"/>
+      <c r="J166" s="368"/>
       <c r="K166" s="116"/>
     </row>
     <row r="167" spans="1:11">
@@ -34569,8 +34575,8 @@
         <v>71</v>
       </c>
       <c r="H167" s="190"/>
-      <c r="I167" s="353"/>
-      <c r="J167" s="395"/>
+      <c r="I167" s="407"/>
+      <c r="J167" s="385"/>
       <c r="K167" s="127"/>
     </row>
     <row r="168" spans="1:11">
@@ -34594,8 +34600,8 @@
         <v>73</v>
       </c>
       <c r="H168" s="190"/>
-      <c r="I168" s="353"/>
-      <c r="J168" s="395"/>
+      <c r="I168" s="407"/>
+      <c r="J168" s="385"/>
       <c r="K168" s="127"/>
     </row>
     <row r="169" spans="1:11" ht="75">
@@ -34619,8 +34625,8 @@
         <v>21</v>
       </c>
       <c r="H169" s="266"/>
-      <c r="I169" s="353"/>
-      <c r="J169" s="395"/>
+      <c r="I169" s="407"/>
+      <c r="J169" s="385"/>
       <c r="K169" s="127"/>
     </row>
     <row r="170" spans="1:11" ht="30">
@@ -34644,8 +34650,8 @@
         <v>75</v>
       </c>
       <c r="H170" s="190"/>
-      <c r="I170" s="353"/>
-      <c r="J170" s="395"/>
+      <c r="I170" s="407"/>
+      <c r="J170" s="385"/>
       <c r="K170" s="127"/>
     </row>
     <row r="171" spans="1:11" ht="45">
@@ -34669,8 +34675,8 @@
         <v>77</v>
       </c>
       <c r="H171" s="190"/>
-      <c r="I171" s="354"/>
-      <c r="J171" s="395"/>
+      <c r="I171" s="408"/>
+      <c r="J171" s="385"/>
       <c r="K171" s="127"/>
     </row>
     <row r="172" spans="1:11" ht="105">
@@ -34694,8 +34700,8 @@
         <v>523</v>
       </c>
       <c r="H172" s="191"/>
-      <c r="I172" s="354"/>
-      <c r="J172" s="395"/>
+      <c r="I172" s="408"/>
+      <c r="J172" s="385"/>
       <c r="K172" s="199"/>
     </row>
     <row r="173" spans="1:11" ht="60">
@@ -34719,8 +34725,8 @@
         <v>227</v>
       </c>
       <c r="H173" s="112"/>
-      <c r="I173" s="355"/>
-      <c r="J173" s="396"/>
+      <c r="I173" s="409"/>
+      <c r="J173" s="386"/>
       <c r="K173" s="116"/>
     </row>
     <row r="174" spans="1:11">
@@ -34759,7 +34765,7 @@
       <c r="H175" s="192" t="s">
         <v>26</v>
       </c>
-      <c r="I175" s="380" t="s">
+      <c r="I175" s="360" t="s">
         <v>6774</v>
       </c>
       <c r="J175" s="192"/>
@@ -34788,7 +34794,7 @@
       <c r="H176" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="I176" s="397"/>
+      <c r="I176" s="387"/>
       <c r="J176" s="193"/>
       <c r="K176" s="193"/>
     </row>
@@ -34815,7 +34821,7 @@
       <c r="H177" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="I177" s="397"/>
+      <c r="I177" s="387"/>
       <c r="J177" s="127"/>
       <c r="K177" s="127"/>
     </row>
@@ -34842,7 +34848,7 @@
       <c r="H178" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="I178" s="397"/>
+      <c r="I178" s="387"/>
       <c r="J178" s="193"/>
       <c r="K178" s="193"/>
     </row>
@@ -34867,7 +34873,7 @@
         <v>77</v>
       </c>
       <c r="H179" s="193"/>
-      <c r="I179" s="351"/>
+      <c r="I179" s="361"/>
       <c r="J179" s="193"/>
       <c r="K179" s="127"/>
     </row>
@@ -34892,7 +34898,7 @@
         <v>523</v>
       </c>
       <c r="H180" s="193"/>
-      <c r="I180" s="351"/>
+      <c r="I180" s="361"/>
       <c r="J180" s="193"/>
       <c r="K180" s="127"/>
     </row>
@@ -34917,7 +34923,7 @@
         <v>227</v>
       </c>
       <c r="H181" s="198"/>
-      <c r="I181" s="351"/>
+      <c r="I181" s="361"/>
       <c r="J181" s="193"/>
       <c r="K181" s="116"/>
     </row>
@@ -34957,10 +34963,10 @@
       <c r="H183" s="197" t="s">
         <v>26</v>
       </c>
-      <c r="I183" s="367" t="s">
+      <c r="I183" s="370" t="s">
         <v>6775</v>
       </c>
-      <c r="J183" s="349"/>
+      <c r="J183" s="401"/>
       <c r="K183" s="197"/>
     </row>
     <row r="184" spans="1:11" ht="45">
@@ -34986,8 +34992,8 @@
       <c r="H184" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="I184" s="376"/>
-      <c r="J184" s="350"/>
+      <c r="I184" s="388"/>
+      <c r="J184" s="405"/>
       <c r="K184" s="198"/>
     </row>
     <row r="185" spans="1:11" ht="45">
@@ -35013,8 +35019,8 @@
       <c r="H185" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="I185" s="376"/>
-      <c r="J185" s="350"/>
+      <c r="I185" s="388"/>
+      <c r="J185" s="405"/>
       <c r="K185" s="116"/>
     </row>
     <row r="186" spans="1:11" ht="45">
@@ -35040,8 +35046,8 @@
       <c r="H186" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="I186" s="376"/>
-      <c r="J186" s="350"/>
+      <c r="I186" s="388"/>
+      <c r="J186" s="405"/>
       <c r="K186" s="198"/>
     </row>
     <row r="187" spans="1:11" ht="48.75" customHeight="1">
@@ -35067,8 +35073,8 @@
       <c r="H187" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="I187" s="358"/>
-      <c r="J187" s="351"/>
+      <c r="I187" s="369"/>
+      <c r="J187" s="361"/>
       <c r="K187" s="116"/>
     </row>
     <row r="188" spans="1:11" ht="30">
@@ -35094,8 +35100,8 @@
       <c r="H188" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="I188" s="358"/>
-      <c r="J188" s="351"/>
+      <c r="I188" s="369"/>
+      <c r="J188" s="361"/>
       <c r="K188" s="198"/>
     </row>
     <row r="189" spans="1:11" ht="30">
@@ -35119,7 +35125,7 @@
         <v>77</v>
       </c>
       <c r="H189" s="193"/>
-      <c r="I189" s="358"/>
+      <c r="I189" s="369"/>
       <c r="J189" s="193"/>
       <c r="K189" s="127"/>
     </row>
@@ -35144,7 +35150,7 @@
         <v>523</v>
       </c>
       <c r="H190" s="193"/>
-      <c r="I190" s="358"/>
+      <c r="I190" s="369"/>
       <c r="J190" s="193"/>
       <c r="K190" s="127"/>
     </row>
@@ -35169,7 +35175,7 @@
         <v>227</v>
       </c>
       <c r="H191" s="198"/>
-      <c r="I191" s="359"/>
+      <c r="I191" s="365"/>
       <c r="J191" s="193"/>
       <c r="K191" s="116"/>
     </row>
@@ -35209,7 +35215,7 @@
       <c r="H193" s="272" t="s">
         <v>26</v>
       </c>
-      <c r="I193" s="371" t="s">
+      <c r="I193" s="362" t="s">
         <v>180</v>
       </c>
       <c r="J193" s="273"/>
@@ -35238,7 +35244,7 @@
       <c r="H194" s="276" t="s">
         <v>26</v>
       </c>
-      <c r="I194" s="372"/>
+      <c r="I194" s="363"/>
       <c r="J194" s="275"/>
       <c r="K194" s="275"/>
     </row>
@@ -35278,7 +35284,7 @@
       <c r="H196" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="I196" s="357" t="s">
+      <c r="I196" s="364" t="s">
         <v>527</v>
       </c>
       <c r="J196" s="158" t="s">
@@ -35309,7 +35315,7 @@
       <c r="H197" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I197" s="359"/>
+      <c r="I197" s="365"/>
       <c r="J197" s="53"/>
       <c r="K197" s="53"/>
     </row>
@@ -35349,7 +35355,7 @@
       <c r="H199" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="I199" s="392" t="s">
+      <c r="I199" s="382" t="s">
         <v>6244</v>
       </c>
       <c r="J199" s="202" t="s">
@@ -35380,7 +35386,7 @@
       <c r="H200" s="206" t="s">
         <v>26</v>
       </c>
-      <c r="I200" s="393"/>
+      <c r="I200" s="383"/>
       <c r="J200" s="206"/>
       <c r="K200" s="207"/>
     </row>
@@ -35405,12 +35411,12 @@
         <v>124</v>
       </c>
       <c r="H201" s="206"/>
-      <c r="I201" s="393"/>
+      <c r="I201" s="383"/>
       <c r="J201" s="206"/>
       <c r="K201" s="207"/>
     </row>
     <row r="202" spans="1:11" ht="150">
-      <c r="A202" s="422" t="s">
+      <c r="A202" s="352" t="s">
         <v>6846</v>
       </c>
       <c r="B202" s="204">
@@ -35432,7 +35438,7 @@
         <v>6243</v>
       </c>
       <c r="H202" s="206"/>
-      <c r="I202" s="393"/>
+      <c r="I202" s="383"/>
       <c r="J202" s="206"/>
       <c r="K202" s="207"/>
     </row>
@@ -35457,12 +35463,12 @@
         <v>532</v>
       </c>
       <c r="H203" s="206"/>
-      <c r="I203" s="393"/>
+      <c r="I203" s="383"/>
       <c r="J203" s="206"/>
       <c r="K203" s="207"/>
     </row>
     <row r="204" spans="1:11" ht="180">
-      <c r="A204" s="421" t="s">
+      <c r="A204" s="351" t="s">
         <v>6845</v>
       </c>
       <c r="B204" s="204">
@@ -35484,7 +35490,7 @@
         <v>534</v>
       </c>
       <c r="H204" s="206"/>
-      <c r="I204" s="394"/>
+      <c r="I204" s="384"/>
       <c r="J204" s="206"/>
       <c r="K204" s="207"/>
     </row>
@@ -35524,7 +35530,7 @@
       <c r="H206" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I206" s="357" t="s">
+      <c r="I206" s="364" t="s">
         <v>125</v>
       </c>
       <c r="J206" s="3"/>
@@ -35553,7 +35559,7 @@
       <c r="H207" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I207" s="359"/>
+      <c r="I207" s="365"/>
       <c r="J207" s="40"/>
       <c r="K207" s="18"/>
     </row>
@@ -35593,7 +35599,7 @@
       <c r="H209" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I209" s="357" t="s">
+      <c r="I209" s="364" t="s">
         <v>127</v>
       </c>
       <c r="J209" s="3"/>
@@ -35622,7 +35628,7 @@
       <c r="H210" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I210" s="359"/>
+      <c r="I210" s="365"/>
       <c r="J210" s="40"/>
       <c r="K210" s="18"/>
     </row>
@@ -35662,7 +35668,7 @@
       <c r="H212" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I212" s="357" t="s">
+      <c r="I212" s="364" t="s">
         <v>6772</v>
       </c>
       <c r="J212" s="49"/>
@@ -35691,7 +35697,7 @@
       <c r="H213" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I213" s="361"/>
+      <c r="I213" s="374"/>
       <c r="J213" s="25"/>
       <c r="K213" s="24"/>
     </row>
@@ -35718,7 +35724,7 @@
       <c r="H214" s="300" t="s">
         <v>26</v>
       </c>
-      <c r="I214" s="361"/>
+      <c r="I214" s="374"/>
       <c r="J214" s="142"/>
       <c r="K214" s="134"/>
     </row>
@@ -35743,7 +35749,7 @@
         <v>6786</v>
       </c>
       <c r="H215" s="300"/>
-      <c r="I215" s="361"/>
+      <c r="I215" s="374"/>
       <c r="J215" s="142"/>
       <c r="K215" s="134"/>
     </row>
@@ -35768,7 +35774,7 @@
         <v>182</v>
       </c>
       <c r="H216" s="261"/>
-      <c r="I216" s="361"/>
+      <c r="I216" s="374"/>
       <c r="J216" s="40"/>
       <c r="K216" s="261"/>
     </row>
@@ -35793,7 +35799,7 @@
         <v>218</v>
       </c>
       <c r="H217" s="260"/>
-      <c r="I217" s="362"/>
+      <c r="I217" s="373"/>
       <c r="J217" s="260"/>
       <c r="K217" s="260"/>
     </row>
@@ -35833,10 +35839,10 @@
       <c r="H219" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I219" s="357" t="s">
+      <c r="I219" s="364" t="s">
         <v>185</v>
       </c>
-      <c r="J219" s="363" t="s">
+      <c r="J219" s="378" t="s">
         <v>184</v>
       </c>
       <c r="K219" s="26"/>
@@ -35864,8 +35870,8 @@
       <c r="H220" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="I220" s="358"/>
-      <c r="J220" s="358"/>
+      <c r="I220" s="369"/>
+      <c r="J220" s="369"/>
       <c r="K220" s="78"/>
     </row>
     <row r="221" spans="1:11">
@@ -35904,7 +35910,7 @@
       <c r="H222" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I222" s="357" t="s">
+      <c r="I222" s="364" t="s">
         <v>190</v>
       </c>
       <c r="J222" s="20"/>
@@ -35933,7 +35939,7 @@
       <c r="H223" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="I223" s="359"/>
+      <c r="I223" s="365"/>
       <c r="J223" s="68"/>
       <c r="K223" s="69"/>
     </row>
@@ -35973,7 +35979,7 @@
       <c r="H225" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I225" s="357" t="s">
+      <c r="I225" s="364" t="s">
         <v>219</v>
       </c>
       <c r="J225" s="29"/>
@@ -36002,7 +36008,7 @@
       <c r="H226" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I226" s="358"/>
+      <c r="I226" s="369"/>
       <c r="J226" s="76" t="s">
         <v>193</v>
       </c>
@@ -36031,7 +36037,7 @@
       <c r="H227" s="276" t="s">
         <v>26</v>
       </c>
-      <c r="I227" s="358"/>
+      <c r="I227" s="369"/>
       <c r="J227" s="54"/>
       <c r="K227" s="53"/>
     </row>
@@ -36058,7 +36064,7 @@
       <c r="H228" s="276" t="s">
         <v>6</v>
       </c>
-      <c r="I228" s="358"/>
+      <c r="I228" s="369"/>
       <c r="J228" s="54"/>
       <c r="K228" s="53"/>
     </row>
@@ -36085,7 +36091,7 @@
       <c r="H229" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I229" s="358"/>
+      <c r="I229" s="369"/>
       <c r="J229" s="54"/>
       <c r="K229" s="53"/>
     </row>
@@ -36112,7 +36118,7 @@
       <c r="H230" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I230" s="359"/>
+      <c r="I230" s="365"/>
       <c r="J230" s="25"/>
       <c r="K230" s="24"/>
     </row>
@@ -36150,7 +36156,7 @@
       <c r="H232" s="168" t="s">
         <v>66</v>
       </c>
-      <c r="I232" s="357" t="s">
+      <c r="I232" s="364" t="s">
         <v>6806</v>
       </c>
       <c r="J232" s="168"/>
@@ -36179,12 +36185,12 @@
       <c r="H233" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="I233" s="360"/>
+      <c r="I233" s="368"/>
       <c r="J233" s="127"/>
       <c r="K233" s="127"/>
     </row>
     <row r="234" spans="1:11" ht="60">
-      <c r="A234" s="420" t="s">
+      <c r="A234" s="350" t="s">
         <v>6807</v>
       </c>
       <c r="B234" s="176" t="s">
@@ -36208,7 +36214,7 @@
       <c r="H234" s="169" t="s">
         <v>5569</v>
       </c>
-      <c r="I234" s="389"/>
+      <c r="I234" s="379"/>
       <c r="J234" s="127"/>
       <c r="K234" s="127"/>
     </row>
@@ -36248,7 +36254,7 @@
       <c r="H236" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I236" s="380" t="s">
+      <c r="I236" s="360" t="s">
         <v>515</v>
       </c>
       <c r="J236" s="50"/>
@@ -36277,7 +36283,7 @@
       <c r="H237" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="I237" s="351"/>
+      <c r="I237" s="361"/>
       <c r="J237" s="129"/>
       <c r="K237" s="129"/>
     </row>
@@ -36347,10 +36353,10 @@
       <c r="H241" s="285" t="s">
         <v>6</v>
       </c>
-      <c r="I241" s="367" t="s">
+      <c r="I241" s="370" t="s">
         <v>6782</v>
       </c>
-      <c r="J241" s="386"/>
+      <c r="J241" s="375"/>
       <c r="K241" s="286"/>
     </row>
     <row r="242" spans="1:11" ht="30">
@@ -36374,8 +36380,8 @@
         <v>6780</v>
       </c>
       <c r="H242" s="185"/>
-      <c r="I242" s="385"/>
-      <c r="J242" s="387"/>
+      <c r="I242" s="371"/>
+      <c r="J242" s="376"/>
       <c r="K242" s="291"/>
     </row>
     <row r="243" spans="1:11">
@@ -36401,8 +36407,8 @@
       <c r="H243" s="282" t="s">
         <v>6</v>
       </c>
-      <c r="I243" s="365"/>
-      <c r="J243" s="388"/>
+      <c r="I243" s="372"/>
+      <c r="J243" s="377"/>
       <c r="K243" s="277"/>
     </row>
     <row r="244" spans="1:11" ht="180">
@@ -36420,7 +36426,7 @@
         <v>35</v>
       </c>
       <c r="F244" s="346" t="s">
-        <v>6852</v>
+        <v>6851</v>
       </c>
       <c r="G244" s="293" t="s">
         <v>6770</v>
@@ -36428,7 +36434,7 @@
       <c r="H244" s="262" t="s">
         <v>6</v>
       </c>
-      <c r="I244" s="362"/>
+      <c r="I244" s="373"/>
       <c r="J244" s="278"/>
       <c r="K244" s="116"/>
     </row>
@@ -36440,12 +36446,59 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="J183:J188"/>
+    <mergeCell ref="I164:I173"/>
+    <mergeCell ref="J84:J89"/>
+    <mergeCell ref="J156:J158"/>
+    <mergeCell ref="I131:I133"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="I141:I146"/>
+    <mergeCell ref="J123:J124"/>
+    <mergeCell ref="I122:I126"/>
+    <mergeCell ref="J117:J120"/>
+    <mergeCell ref="I117:I120"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="J99:J106"/>
+    <mergeCell ref="I152:I153"/>
+    <mergeCell ref="I99:I106"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="I113:I115"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="I135:I136"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="I70:I77"/>
+    <mergeCell ref="I79:I82"/>
+    <mergeCell ref="I94:I97"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="I63:I65"/>
+    <mergeCell ref="J63:J65"/>
+    <mergeCell ref="J70:J77"/>
+    <mergeCell ref="J79:J82"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="I67:I68"/>
+    <mergeCell ref="I84:I89"/>
+    <mergeCell ref="I160:I162"/>
+    <mergeCell ref="I241:I244"/>
+    <mergeCell ref="I212:I217"/>
+    <mergeCell ref="J241:J243"/>
+    <mergeCell ref="I225:I230"/>
+    <mergeCell ref="I219:I220"/>
+    <mergeCell ref="I222:I223"/>
+    <mergeCell ref="J219:J220"/>
+    <mergeCell ref="I232:I234"/>
+    <mergeCell ref="J160:J162"/>
+    <mergeCell ref="I236:I237"/>
+    <mergeCell ref="I196:I197"/>
+    <mergeCell ref="I199:I204"/>
+    <mergeCell ref="J165:J173"/>
+    <mergeCell ref="I175:I181"/>
+    <mergeCell ref="I183:I191"/>
     <mergeCell ref="I156:I158"/>
     <mergeCell ref="I193:I194"/>
     <mergeCell ref="I206:I207"/>
@@ -36462,59 +36515,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I160:I162"/>
-    <mergeCell ref="I241:I244"/>
-    <mergeCell ref="I212:I217"/>
-    <mergeCell ref="J241:J243"/>
-    <mergeCell ref="I225:I230"/>
-    <mergeCell ref="I219:I220"/>
-    <mergeCell ref="I222:I223"/>
-    <mergeCell ref="J219:J220"/>
-    <mergeCell ref="I232:I234"/>
-    <mergeCell ref="J160:J162"/>
-    <mergeCell ref="I236:I237"/>
-    <mergeCell ref="I196:I197"/>
-    <mergeCell ref="I199:I204"/>
-    <mergeCell ref="J165:J173"/>
-    <mergeCell ref="I175:I181"/>
-    <mergeCell ref="I183:I191"/>
-    <mergeCell ref="I135:I136"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="I70:I77"/>
-    <mergeCell ref="I79:I82"/>
-    <mergeCell ref="I94:I97"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="I63:I65"/>
-    <mergeCell ref="J63:J65"/>
-    <mergeCell ref="J70:J77"/>
-    <mergeCell ref="J79:J82"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="I67:I68"/>
-    <mergeCell ref="I84:I89"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="E103:E106"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="I113:I115"/>
-    <mergeCell ref="F103:F106"/>
-    <mergeCell ref="J183:J188"/>
-    <mergeCell ref="I164:I173"/>
-    <mergeCell ref="J84:J89"/>
-    <mergeCell ref="J156:J158"/>
-    <mergeCell ref="I131:I133"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="I141:I146"/>
-    <mergeCell ref="J123:J124"/>
-    <mergeCell ref="I122:I126"/>
-    <mergeCell ref="J117:J120"/>
-    <mergeCell ref="I117:I120"/>
-    <mergeCell ref="I91:I92"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="J99:J106"/>
-    <mergeCell ref="I152:I153"/>
-    <mergeCell ref="I99:I106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36638,196 +36644,196 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="65.25" customHeight="1">
-      <c r="A3" s="407" t="s">
+      <c r="A3" s="411" t="s">
         <v>6210</v>
       </c>
       <c r="B3" s="154" t="s">
         <v>6143</v>
       </c>
-      <c r="C3" s="407" t="s">
+      <c r="C3" s="411" t="s">
         <v>6211</v>
       </c>
-      <c r="D3" s="409"/>
-      <c r="E3" s="409"/>
-      <c r="F3" s="405" t="s">
+      <c r="D3" s="412"/>
+      <c r="E3" s="412"/>
+      <c r="F3" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="405" t="s">
+      <c r="G3" s="413" t="s">
         <v>6149</v>
       </c>
       <c r="H3" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="407" t="s">
+      <c r="I3" s="411" t="s">
         <v>6218</v>
       </c>
-      <c r="J3" s="409"/>
-      <c r="K3" s="409"/>
-      <c r="L3" s="409"/>
-      <c r="M3" s="407" t="s">
+      <c r="J3" s="412"/>
+      <c r="K3" s="412"/>
+      <c r="L3" s="412"/>
+      <c r="M3" s="411" t="s">
         <v>6212</v>
       </c>
-      <c r="N3" s="407" t="s">
+      <c r="N3" s="411" t="s">
         <v>6213</v>
       </c>
-      <c r="O3" s="407" t="s">
+      <c r="O3" s="411" t="s">
         <v>6214</v>
       </c>
-      <c r="P3" s="405" t="s">
+      <c r="P3" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="Q3" s="405" t="s">
+      <c r="Q3" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="407" t="s">
+      <c r="R3" s="411" t="s">
         <v>6215</v>
       </c>
-      <c r="S3" s="407" t="s">
+      <c r="S3" s="411" t="s">
         <v>6216</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1">
-      <c r="A4" s="407"/>
+      <c r="A4" s="411"/>
       <c r="B4" s="154" t="s">
         <v>6144</v>
       </c>
-      <c r="C4" s="409"/>
-      <c r="D4" s="409"/>
-      <c r="E4" s="409"/>
-      <c r="F4" s="406"/>
-      <c r="G4" s="406"/>
+      <c r="C4" s="412"/>
+      <c r="D4" s="412"/>
+      <c r="E4" s="412"/>
+      <c r="F4" s="415"/>
+      <c r="G4" s="415"/>
       <c r="H4" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="I4" s="409"/>
-      <c r="J4" s="409"/>
-      <c r="K4" s="409"/>
-      <c r="L4" s="409"/>
-      <c r="M4" s="409"/>
-      <c r="N4" s="409"/>
-      <c r="O4" s="409"/>
-      <c r="P4" s="405"/>
-      <c r="Q4" s="405"/>
-      <c r="R4" s="409"/>
-      <c r="S4" s="409"/>
+      <c r="I4" s="412"/>
+      <c r="J4" s="412"/>
+      <c r="K4" s="412"/>
+      <c r="L4" s="412"/>
+      <c r="M4" s="412"/>
+      <c r="N4" s="412"/>
+      <c r="O4" s="412"/>
+      <c r="P4" s="413"/>
+      <c r="Q4" s="413"/>
+      <c r="R4" s="412"/>
+      <c r="S4" s="412"/>
     </row>
     <row r="5" spans="1:19" ht="66.75" customHeight="1">
-      <c r="A5" s="407"/>
+      <c r="A5" s="411"/>
       <c r="B5" s="154" t="s">
         <v>6145</v>
       </c>
-      <c r="C5" s="409"/>
-      <c r="D5" s="409"/>
-      <c r="E5" s="409"/>
-      <c r="F5" s="406"/>
-      <c r="G5" s="406"/>
+      <c r="C5" s="412"/>
+      <c r="D5" s="412"/>
+      <c r="E5" s="412"/>
+      <c r="F5" s="415"/>
+      <c r="G5" s="415"/>
       <c r="H5" s="155" t="s">
         <v>6084</v>
       </c>
-      <c r="I5" s="409"/>
-      <c r="J5" s="409"/>
-      <c r="K5" s="409"/>
-      <c r="L5" s="409"/>
-      <c r="M5" s="409"/>
-      <c r="N5" s="409"/>
-      <c r="O5" s="409"/>
-      <c r="P5" s="405"/>
-      <c r="Q5" s="405"/>
-      <c r="R5" s="409"/>
-      <c r="S5" s="409"/>
+      <c r="I5" s="412"/>
+      <c r="J5" s="412"/>
+      <c r="K5" s="412"/>
+      <c r="L5" s="412"/>
+      <c r="M5" s="412"/>
+      <c r="N5" s="412"/>
+      <c r="O5" s="412"/>
+      <c r="P5" s="413"/>
+      <c r="Q5" s="413"/>
+      <c r="R5" s="412"/>
+      <c r="S5" s="412"/>
     </row>
     <row r="6" spans="1:19" ht="66.75" customHeight="1">
-      <c r="A6" s="407"/>
+      <c r="A6" s="411"/>
       <c r="B6" s="154" t="s">
         <v>6146</v>
       </c>
-      <c r="C6" s="409"/>
-      <c r="D6" s="409"/>
-      <c r="E6" s="409"/>
-      <c r="F6" s="406"/>
-      <c r="G6" s="406"/>
+      <c r="C6" s="412"/>
+      <c r="D6" s="412"/>
+      <c r="E6" s="412"/>
+      <c r="F6" s="415"/>
+      <c r="G6" s="415"/>
       <c r="H6" s="155" t="s">
         <v>228</v>
       </c>
-      <c r="I6" s="409"/>
-      <c r="J6" s="409"/>
-      <c r="K6" s="409"/>
-      <c r="L6" s="409"/>
-      <c r="M6" s="409"/>
-      <c r="N6" s="409"/>
-      <c r="O6" s="409"/>
-      <c r="P6" s="405"/>
-      <c r="Q6" s="405"/>
-      <c r="R6" s="409"/>
-      <c r="S6" s="409"/>
+      <c r="I6" s="412"/>
+      <c r="J6" s="412"/>
+      <c r="K6" s="412"/>
+      <c r="L6" s="412"/>
+      <c r="M6" s="412"/>
+      <c r="N6" s="412"/>
+      <c r="O6" s="412"/>
+      <c r="P6" s="413"/>
+      <c r="Q6" s="413"/>
+      <c r="R6" s="412"/>
+      <c r="S6" s="412"/>
     </row>
     <row r="7" spans="1:19" ht="72.75" customHeight="1">
-      <c r="A7" s="407"/>
+      <c r="A7" s="411"/>
       <c r="B7" s="154" t="s">
         <v>6147</v>
       </c>
-      <c r="C7" s="409"/>
-      <c r="D7" s="409"/>
-      <c r="E7" s="409"/>
-      <c r="F7" s="406"/>
-      <c r="G7" s="406"/>
+      <c r="C7" s="412"/>
+      <c r="D7" s="412"/>
+      <c r="E7" s="412"/>
+      <c r="F7" s="415"/>
+      <c r="G7" s="415"/>
       <c r="H7" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="I7" s="409"/>
-      <c r="J7" s="409"/>
-      <c r="K7" s="409"/>
-      <c r="L7" s="409"/>
-      <c r="M7" s="409"/>
-      <c r="N7" s="409"/>
-      <c r="O7" s="409"/>
-      <c r="P7" s="405"/>
-      <c r="Q7" s="405"/>
-      <c r="R7" s="409"/>
-      <c r="S7" s="409"/>
+      <c r="I7" s="412"/>
+      <c r="J7" s="412"/>
+      <c r="K7" s="412"/>
+      <c r="L7" s="412"/>
+      <c r="M7" s="412"/>
+      <c r="N7" s="412"/>
+      <c r="O7" s="412"/>
+      <c r="P7" s="413"/>
+      <c r="Q7" s="413"/>
+      <c r="R7" s="412"/>
+      <c r="S7" s="412"/>
     </row>
     <row r="8" spans="1:19" ht="72.75" customHeight="1">
-      <c r="A8" s="407"/>
+      <c r="A8" s="411"/>
       <c r="B8" s="154" t="s">
         <v>6148</v>
       </c>
-      <c r="C8" s="409"/>
-      <c r="D8" s="409"/>
-      <c r="E8" s="409"/>
-      <c r="F8" s="406"/>
-      <c r="G8" s="406"/>
+      <c r="C8" s="412"/>
+      <c r="D8" s="412"/>
+      <c r="E8" s="412"/>
+      <c r="F8" s="415"/>
+      <c r="G8" s="415"/>
       <c r="H8" s="155" t="s">
         <v>6150</v>
       </c>
-      <c r="I8" s="409"/>
-      <c r="J8" s="409"/>
-      <c r="K8" s="409"/>
-      <c r="L8" s="409"/>
-      <c r="M8" s="409"/>
-      <c r="N8" s="409"/>
-      <c r="O8" s="409"/>
-      <c r="P8" s="405"/>
-      <c r="Q8" s="405"/>
-      <c r="R8" s="409"/>
-      <c r="S8" s="409"/>
+      <c r="I8" s="412"/>
+      <c r="J8" s="412"/>
+      <c r="K8" s="412"/>
+      <c r="L8" s="412"/>
+      <c r="M8" s="412"/>
+      <c r="N8" s="412"/>
+      <c r="O8" s="412"/>
+      <c r="P8" s="413"/>
+      <c r="Q8" s="413"/>
+      <c r="R8" s="412"/>
+      <c r="S8" s="412"/>
     </row>
     <row r="9" spans="1:19" ht="78" customHeight="1">
-      <c r="A9" s="407" t="s">
+      <c r="A9" s="411" t="s">
         <v>6219</v>
       </c>
       <c r="B9" s="154" t="s">
         <v>6143</v>
       </c>
-      <c r="C9" s="407" t="s">
+      <c r="C9" s="411" t="s">
         <v>6158</v>
       </c>
-      <c r="D9" s="407" t="s">
+      <c r="D9" s="411" t="s">
         <v>6159</v>
       </c>
-      <c r="E9" s="405" t="s">
+      <c r="E9" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="405" t="s">
+      <c r="F9" s="413" t="s">
         <v>6149</v>
       </c>
       <c r="G9" s="155" t="s">
@@ -36836,299 +36842,299 @@
       <c r="H9" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="405" t="s">
+      <c r="I9" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="J9" s="407" t="s">
+      <c r="J9" s="411" t="s">
         <v>6217</v>
       </c>
-      <c r="K9" s="408"/>
-      <c r="L9" s="408"/>
-      <c r="M9" s="409"/>
-      <c r="N9" s="408"/>
-      <c r="O9" s="410" t="s">
+      <c r="K9" s="416"/>
+      <c r="L9" s="416"/>
+      <c r="M9" s="412"/>
+      <c r="N9" s="416"/>
+      <c r="O9" s="417" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="405" t="s">
+      <c r="P9" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="405"/>
-      <c r="R9" s="407" t="s">
+      <c r="Q9" s="413"/>
+      <c r="R9" s="411" t="s">
         <v>6162</v>
       </c>
-      <c r="S9" s="405" t="s">
+      <c r="S9" s="413" t="s">
         <v>6149</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="75.75" customHeight="1">
-      <c r="A10" s="407"/>
+      <c r="A10" s="411"/>
       <c r="B10" s="154" t="s">
         <v>6144</v>
       </c>
-      <c r="C10" s="407"/>
-      <c r="D10" s="407"/>
-      <c r="E10" s="405"/>
-      <c r="F10" s="405"/>
+      <c r="C10" s="411"/>
+      <c r="D10" s="411"/>
+      <c r="E10" s="413"/>
+      <c r="F10" s="413"/>
       <c r="G10" s="155" t="s">
         <v>267</v>
       </c>
       <c r="H10" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="I10" s="406"/>
-      <c r="J10" s="408"/>
-      <c r="K10" s="408"/>
-      <c r="L10" s="408"/>
-      <c r="M10" s="409"/>
-      <c r="N10" s="408"/>
-      <c r="O10" s="410"/>
-      <c r="P10" s="405"/>
-      <c r="Q10" s="405"/>
-      <c r="R10" s="381"/>
-      <c r="S10" s="408"/>
+      <c r="I10" s="415"/>
+      <c r="J10" s="416"/>
+      <c r="K10" s="416"/>
+      <c r="L10" s="416"/>
+      <c r="M10" s="412"/>
+      <c r="N10" s="416"/>
+      <c r="O10" s="417"/>
+      <c r="P10" s="413"/>
+      <c r="Q10" s="413"/>
+      <c r="R10" s="395"/>
+      <c r="S10" s="416"/>
     </row>
     <row r="11" spans="1:19" ht="75" customHeight="1">
-      <c r="A11" s="407"/>
+      <c r="A11" s="411"/>
       <c r="B11" s="154" t="s">
         <v>6145</v>
       </c>
-      <c r="C11" s="407"/>
-      <c r="D11" s="407"/>
-      <c r="E11" s="405"/>
-      <c r="F11" s="405"/>
+      <c r="C11" s="411"/>
+      <c r="D11" s="411"/>
+      <c r="E11" s="413"/>
+      <c r="F11" s="413"/>
       <c r="G11" s="155" t="s">
         <v>6084</v>
       </c>
       <c r="H11" s="155" t="s">
         <v>6084</v>
       </c>
-      <c r="I11" s="406"/>
-      <c r="J11" s="408"/>
-      <c r="K11" s="408"/>
-      <c r="L11" s="408"/>
-      <c r="M11" s="409"/>
-      <c r="N11" s="408"/>
-      <c r="O11" s="410"/>
-      <c r="P11" s="405"/>
-      <c r="Q11" s="405"/>
-      <c r="R11" s="381"/>
-      <c r="S11" s="408"/>
+      <c r="I11" s="415"/>
+      <c r="J11" s="416"/>
+      <c r="K11" s="416"/>
+      <c r="L11" s="416"/>
+      <c r="M11" s="412"/>
+      <c r="N11" s="416"/>
+      <c r="O11" s="417"/>
+      <c r="P11" s="413"/>
+      <c r="Q11" s="413"/>
+      <c r="R11" s="395"/>
+      <c r="S11" s="416"/>
     </row>
     <row r="12" spans="1:19" ht="65.25" customHeight="1">
-      <c r="A12" s="407"/>
+      <c r="A12" s="411"/>
       <c r="B12" s="154" t="s">
         <v>6146</v>
       </c>
-      <c r="C12" s="407"/>
-      <c r="D12" s="407"/>
-      <c r="E12" s="406"/>
-      <c r="F12" s="405"/>
+      <c r="C12" s="411"/>
+      <c r="D12" s="411"/>
+      <c r="E12" s="415"/>
+      <c r="F12" s="413"/>
       <c r="G12" s="155" t="s">
         <v>228</v>
       </c>
       <c r="H12" s="155" t="s">
         <v>228</v>
       </c>
-      <c r="I12" s="406"/>
-      <c r="J12" s="408"/>
-      <c r="K12" s="408"/>
-      <c r="L12" s="408"/>
-      <c r="M12" s="409"/>
-      <c r="N12" s="408"/>
-      <c r="O12" s="410"/>
-      <c r="P12" s="406"/>
-      <c r="Q12" s="405"/>
-      <c r="R12" s="381"/>
-      <c r="S12" s="408"/>
+      <c r="I12" s="415"/>
+      <c r="J12" s="416"/>
+      <c r="K12" s="416"/>
+      <c r="L12" s="416"/>
+      <c r="M12" s="412"/>
+      <c r="N12" s="416"/>
+      <c r="O12" s="417"/>
+      <c r="P12" s="415"/>
+      <c r="Q12" s="413"/>
+      <c r="R12" s="395"/>
+      <c r="S12" s="416"/>
     </row>
     <row r="13" spans="1:19" ht="63" customHeight="1">
-      <c r="A13" s="407"/>
+      <c r="A13" s="411"/>
       <c r="B13" s="154" t="s">
         <v>6147</v>
       </c>
-      <c r="C13" s="407"/>
-      <c r="D13" s="407"/>
-      <c r="E13" s="406"/>
-      <c r="F13" s="406"/>
+      <c r="C13" s="411"/>
+      <c r="D13" s="411"/>
+      <c r="E13" s="415"/>
+      <c r="F13" s="415"/>
       <c r="G13" s="155" t="s">
         <v>267</v>
       </c>
       <c r="H13" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="I13" s="406"/>
-      <c r="J13" s="408"/>
-      <c r="K13" s="408"/>
-      <c r="L13" s="408"/>
-      <c r="M13" s="409"/>
-      <c r="N13" s="408"/>
-      <c r="O13" s="411"/>
-      <c r="P13" s="406"/>
-      <c r="Q13" s="405"/>
-      <c r="R13" s="381"/>
-      <c r="S13" s="408"/>
+      <c r="I13" s="415"/>
+      <c r="J13" s="416"/>
+      <c r="K13" s="416"/>
+      <c r="L13" s="416"/>
+      <c r="M13" s="412"/>
+      <c r="N13" s="416"/>
+      <c r="O13" s="418"/>
+      <c r="P13" s="415"/>
+      <c r="Q13" s="413"/>
+      <c r="R13" s="395"/>
+      <c r="S13" s="416"/>
     </row>
     <row r="14" spans="1:19" ht="51" customHeight="1">
-      <c r="A14" s="407"/>
+      <c r="A14" s="411"/>
       <c r="B14" s="154" t="s">
         <v>6148</v>
       </c>
-      <c r="C14" s="407"/>
-      <c r="D14" s="407"/>
-      <c r="E14" s="406"/>
-      <c r="F14" s="406"/>
+      <c r="C14" s="411"/>
+      <c r="D14" s="411"/>
+      <c r="E14" s="415"/>
+      <c r="F14" s="415"/>
       <c r="G14" s="155" t="s">
         <v>6150</v>
       </c>
       <c r="H14" s="155" t="s">
         <v>6150</v>
       </c>
-      <c r="I14" s="406"/>
-      <c r="J14" s="408"/>
-      <c r="K14" s="408"/>
-      <c r="L14" s="408"/>
-      <c r="M14" s="409"/>
-      <c r="N14" s="408"/>
-      <c r="O14" s="411"/>
-      <c r="P14" s="406"/>
-      <c r="Q14" s="405"/>
-      <c r="R14" s="381"/>
-      <c r="S14" s="408"/>
+      <c r="I14" s="415"/>
+      <c r="J14" s="416"/>
+      <c r="K14" s="416"/>
+      <c r="L14" s="416"/>
+      <c r="M14" s="412"/>
+      <c r="N14" s="416"/>
+      <c r="O14" s="418"/>
+      <c r="P14" s="415"/>
+      <c r="Q14" s="413"/>
+      <c r="R14" s="395"/>
+      <c r="S14" s="416"/>
     </row>
     <row r="15" spans="1:19" ht="33.950000000000003" customHeight="1">
-      <c r="A15" s="407" t="s">
+      <c r="A15" s="411" t="s">
         <v>6220</v>
       </c>
       <c r="B15" s="154" t="s">
         <v>6151</v>
       </c>
-      <c r="C15" s="405" t="s">
+      <c r="C15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="405" t="s">
+      <c r="D15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="406"/>
-      <c r="F15" s="405" t="s">
+      <c r="E15" s="415"/>
+      <c r="F15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="405" t="s">
+      <c r="G15" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="H15" s="405" t="s">
+      <c r="H15" s="413" t="s">
         <v>6075</v>
       </c>
-      <c r="I15" s="405" t="s">
+      <c r="I15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="405" t="s">
+      <c r="J15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="405" t="s">
+      <c r="K15" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="L15" s="405" t="s">
+      <c r="L15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="409"/>
-      <c r="N15" s="405" t="s">
+      <c r="M15" s="412"/>
+      <c r="N15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="411"/>
-      <c r="P15" s="406"/>
-      <c r="Q15" s="405"/>
-      <c r="R15" s="405" t="s">
+      <c r="O15" s="418"/>
+      <c r="P15" s="415"/>
+      <c r="Q15" s="413"/>
+      <c r="R15" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="S15" s="405" t="s">
+      <c r="S15" s="413" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="33.950000000000003" customHeight="1">
-      <c r="A16" s="407"/>
+      <c r="A16" s="411"/>
       <c r="B16" s="154" t="s">
         <v>6152</v>
       </c>
-      <c r="C16" s="405"/>
-      <c r="D16" s="405"/>
-      <c r="E16" s="406"/>
-      <c r="F16" s="405"/>
-      <c r="G16" s="406"/>
-      <c r="H16" s="405"/>
-      <c r="I16" s="405"/>
-      <c r="J16" s="405"/>
-      <c r="K16" s="405"/>
-      <c r="L16" s="405"/>
-      <c r="M16" s="409"/>
-      <c r="N16" s="405"/>
-      <c r="O16" s="411"/>
-      <c r="P16" s="406"/>
-      <c r="Q16" s="405"/>
-      <c r="R16" s="405"/>
-      <c r="S16" s="405"/>
+      <c r="C16" s="413"/>
+      <c r="D16" s="413"/>
+      <c r="E16" s="415"/>
+      <c r="F16" s="413"/>
+      <c r="G16" s="415"/>
+      <c r="H16" s="413"/>
+      <c r="I16" s="413"/>
+      <c r="J16" s="413"/>
+      <c r="K16" s="413"/>
+      <c r="L16" s="413"/>
+      <c r="M16" s="412"/>
+      <c r="N16" s="413"/>
+      <c r="O16" s="418"/>
+      <c r="P16" s="415"/>
+      <c r="Q16" s="413"/>
+      <c r="R16" s="413"/>
+      <c r="S16" s="413"/>
     </row>
     <row r="17" spans="1:19" ht="33.950000000000003" customHeight="1">
-      <c r="A17" s="407"/>
+      <c r="A17" s="411"/>
       <c r="B17" s="154" t="s">
         <v>6153</v>
       </c>
-      <c r="C17" s="405"/>
-      <c r="D17" s="405"/>
-      <c r="E17" s="406"/>
-      <c r="F17" s="405"/>
-      <c r="G17" s="406"/>
-      <c r="H17" s="405"/>
-      <c r="I17" s="405"/>
-      <c r="J17" s="405"/>
-      <c r="K17" s="405"/>
-      <c r="L17" s="405"/>
-      <c r="M17" s="409"/>
-      <c r="N17" s="405"/>
-      <c r="O17" s="411"/>
-      <c r="P17" s="406"/>
-      <c r="Q17" s="405"/>
-      <c r="R17" s="405"/>
-      <c r="S17" s="405"/>
+      <c r="C17" s="413"/>
+      <c r="D17" s="413"/>
+      <c r="E17" s="415"/>
+      <c r="F17" s="413"/>
+      <c r="G17" s="415"/>
+      <c r="H17" s="413"/>
+      <c r="I17" s="413"/>
+      <c r="J17" s="413"/>
+      <c r="K17" s="413"/>
+      <c r="L17" s="413"/>
+      <c r="M17" s="412"/>
+      <c r="N17" s="413"/>
+      <c r="O17" s="418"/>
+      <c r="P17" s="415"/>
+      <c r="Q17" s="413"/>
+      <c r="R17" s="413"/>
+      <c r="S17" s="413"/>
     </row>
     <row r="18" spans="1:19" ht="33.950000000000003" customHeight="1">
-      <c r="A18" s="407"/>
+      <c r="A18" s="411"/>
       <c r="B18" s="154" t="s">
         <v>6154</v>
       </c>
-      <c r="C18" s="405" t="s">
+      <c r="C18" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="D18" s="405" t="s">
+      <c r="D18" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="E18" s="405" t="s">
+      <c r="E18" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="F18" s="405" t="s">
+      <c r="F18" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="G18" s="406"/>
+      <c r="G18" s="415"/>
       <c r="H18" s="155" t="s">
         <v>6149</v>
       </c>
-      <c r="I18" s="405"/>
-      <c r="J18" s="405" t="s">
+      <c r="I18" s="413"/>
+      <c r="J18" s="413" t="s">
         <v>6149</v>
       </c>
       <c r="K18" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="405"/>
-      <c r="M18" s="409"/>
-      <c r="N18" s="405" t="s">
+      <c r="L18" s="413"/>
+      <c r="M18" s="412"/>
+      <c r="N18" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="O18" s="411"/>
+      <c r="O18" s="418"/>
       <c r="P18" s="155" t="s">
         <v>6149</v>
       </c>
-      <c r="Q18" s="405"/>
-      <c r="R18" s="405" t="s">
+      <c r="Q18" s="413"/>
+      <c r="R18" s="413" t="s">
         <v>6149</v>
       </c>
       <c r="S18" s="155" t="s">
@@ -37136,166 +37142,166 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="166.5" customHeight="1">
-      <c r="A19" s="407"/>
+      <c r="A19" s="411"/>
       <c r="B19" s="154" t="s">
         <v>6155</v>
       </c>
-      <c r="C19" s="405"/>
-      <c r="D19" s="405"/>
-      <c r="E19" s="405"/>
-      <c r="F19" s="405"/>
-      <c r="G19" s="406"/>
-      <c r="H19" s="405" t="s">
+      <c r="C19" s="413"/>
+      <c r="D19" s="413"/>
+      <c r="E19" s="413"/>
+      <c r="F19" s="413"/>
+      <c r="G19" s="415"/>
+      <c r="H19" s="413" t="s">
         <v>6075</v>
       </c>
-      <c r="I19" s="405" t="s">
+      <c r="I19" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="J19" s="405"/>
-      <c r="K19" s="405" t="s">
+      <c r="J19" s="413"/>
+      <c r="K19" s="413" t="s">
         <v>6149</v>
       </c>
-      <c r="L19" s="418" t="s">
+      <c r="L19" s="414" t="s">
         <v>6149</v>
       </c>
-      <c r="M19" s="418" t="s">
+      <c r="M19" s="414" t="s">
         <v>6149</v>
       </c>
-      <c r="N19" s="405"/>
-      <c r="O19" s="407" t="s">
+      <c r="N19" s="413"/>
+      <c r="O19" s="411" t="s">
         <v>6222</v>
       </c>
-      <c r="P19" s="409"/>
-      <c r="Q19" s="405"/>
-      <c r="R19" s="405"/>
-      <c r="S19" s="405" t="s">
+      <c r="P19" s="412"/>
+      <c r="Q19" s="413"/>
+      <c r="R19" s="413"/>
+      <c r="S19" s="413" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="155.25" customHeight="1">
-      <c r="A20" s="407"/>
+      <c r="A20" s="411"/>
       <c r="B20" s="154" t="s">
         <v>6156</v>
       </c>
-      <c r="C20" s="405"/>
-      <c r="D20" s="405"/>
-      <c r="E20" s="405"/>
-      <c r="F20" s="405"/>
-      <c r="G20" s="406"/>
-      <c r="H20" s="405"/>
-      <c r="I20" s="405"/>
-      <c r="J20" s="405"/>
-      <c r="K20" s="405"/>
-      <c r="L20" s="418"/>
-      <c r="M20" s="418"/>
-      <c r="N20" s="405"/>
-      <c r="O20" s="409"/>
-      <c r="P20" s="409"/>
-      <c r="Q20" s="405"/>
-      <c r="R20" s="405"/>
-      <c r="S20" s="405"/>
+      <c r="C20" s="413"/>
+      <c r="D20" s="413"/>
+      <c r="E20" s="413"/>
+      <c r="F20" s="413"/>
+      <c r="G20" s="415"/>
+      <c r="H20" s="413"/>
+      <c r="I20" s="413"/>
+      <c r="J20" s="413"/>
+      <c r="K20" s="413"/>
+      <c r="L20" s="414"/>
+      <c r="M20" s="414"/>
+      <c r="N20" s="413"/>
+      <c r="O20" s="412"/>
+      <c r="P20" s="412"/>
+      <c r="Q20" s="413"/>
+      <c r="R20" s="413"/>
+      <c r="S20" s="413"/>
     </row>
     <row r="21" spans="1:19" ht="149.25" customHeight="1">
-      <c r="A21" s="407"/>
+      <c r="A21" s="411"/>
       <c r="B21" s="154" t="s">
         <v>6157</v>
       </c>
-      <c r="C21" s="405"/>
-      <c r="D21" s="405"/>
-      <c r="E21" s="405"/>
-      <c r="F21" s="405"/>
-      <c r="G21" s="406"/>
-      <c r="H21" s="405"/>
-      <c r="I21" s="405"/>
-      <c r="J21" s="405"/>
-      <c r="K21" s="405"/>
-      <c r="L21" s="418"/>
-      <c r="M21" s="418"/>
-      <c r="N21" s="405"/>
-      <c r="O21" s="409"/>
-      <c r="P21" s="409"/>
-      <c r="Q21" s="405"/>
-      <c r="R21" s="405"/>
-      <c r="S21" s="405"/>
+      <c r="C21" s="413"/>
+      <c r="D21" s="413"/>
+      <c r="E21" s="413"/>
+      <c r="F21" s="413"/>
+      <c r="G21" s="415"/>
+      <c r="H21" s="413"/>
+      <c r="I21" s="413"/>
+      <c r="J21" s="413"/>
+      <c r="K21" s="413"/>
+      <c r="L21" s="414"/>
+      <c r="M21" s="414"/>
+      <c r="N21" s="413"/>
+      <c r="O21" s="412"/>
+      <c r="P21" s="412"/>
+      <c r="Q21" s="413"/>
+      <c r="R21" s="413"/>
+      <c r="S21" s="413"/>
     </row>
     <row r="22" spans="1:19" ht="56.25" customHeight="1">
-      <c r="A22" s="381"/>
+      <c r="A22" s="395"/>
       <c r="B22" s="156" t="s">
         <v>6163</v>
       </c>
-      <c r="C22" s="412" t="s">
+      <c r="C22" s="419" t="s">
         <v>6221</v>
       </c>
-      <c r="D22" s="413"/>
-      <c r="E22" s="414"/>
-      <c r="F22" s="405" t="s">
+      <c r="D22" s="420"/>
+      <c r="E22" s="421"/>
+      <c r="F22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="405" t="s">
+      <c r="G22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="405" t="s">
+      <c r="H22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="405" t="s">
+      <c r="I22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="405" t="s">
+      <c r="J22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="405" t="s">
+      <c r="K22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="405" t="s">
+      <c r="L22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="407" t="s">
+      <c r="M22" s="411" t="s">
         <v>6212</v>
       </c>
-      <c r="N22" s="405" t="s">
+      <c r="N22" s="413" t="s">
         <v>6075</v>
       </c>
-      <c r="O22" s="405" t="s">
+      <c r="O22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="P22" s="405" t="s">
+      <c r="P22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="Q22" s="405" t="s">
+      <c r="Q22" s="413" t="s">
         <v>41</v>
       </c>
-      <c r="R22" s="405" t="s">
+      <c r="R22" s="413" t="s">
         <v>288</v>
       </c>
-      <c r="S22" s="405" t="s">
+      <c r="S22" s="413" t="s">
         <v>6149</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="51.75" customHeight="1">
-      <c r="A23" s="381"/>
+      <c r="A23" s="395"/>
       <c r="B23" s="156" t="s">
         <v>6164</v>
       </c>
-      <c r="C23" s="415"/>
-      <c r="D23" s="416"/>
-      <c r="E23" s="417"/>
-      <c r="F23" s="405"/>
-      <c r="G23" s="405"/>
-      <c r="H23" s="405"/>
-      <c r="I23" s="405"/>
-      <c r="J23" s="405"/>
-      <c r="K23" s="405"/>
-      <c r="L23" s="405"/>
-      <c r="M23" s="381"/>
-      <c r="N23" s="406"/>
-      <c r="O23" s="405"/>
-      <c r="P23" s="405"/>
-      <c r="Q23" s="405"/>
-      <c r="R23" s="406"/>
-      <c r="S23" s="406"/>
+      <c r="C23" s="422"/>
+      <c r="D23" s="423"/>
+      <c r="E23" s="424"/>
+      <c r="F23" s="413"/>
+      <c r="G23" s="413"/>
+      <c r="H23" s="413"/>
+      <c r="I23" s="413"/>
+      <c r="J23" s="413"/>
+      <c r="K23" s="413"/>
+      <c r="L23" s="413"/>
+      <c r="M23" s="395"/>
+      <c r="N23" s="415"/>
+      <c r="O23" s="413"/>
+      <c r="P23" s="413"/>
+      <c r="Q23" s="413"/>
+      <c r="R23" s="415"/>
+      <c r="S23" s="415"/>
     </row>
     <row r="24" spans="1:19" ht="33.950000000000003" customHeight="1">
-      <c r="A24" s="381"/>
+      <c r="A24" s="395"/>
       <c r="B24" s="156" t="s">
         <v>6165</v>
       </c>
@@ -37308,27 +37314,76 @@
       <c r="E24" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="405"/>
-      <c r="G24" s="405"/>
-      <c r="H24" s="405"/>
-      <c r="I24" s="405"/>
-      <c r="J24" s="405"/>
-      <c r="K24" s="405"/>
-      <c r="L24" s="405"/>
-      <c r="M24" s="381"/>
+      <c r="F24" s="413"/>
+      <c r="G24" s="413"/>
+      <c r="H24" s="413"/>
+      <c r="I24" s="413"/>
+      <c r="J24" s="413"/>
+      <c r="K24" s="413"/>
+      <c r="L24" s="413"/>
+      <c r="M24" s="395"/>
       <c r="N24" s="155" t="s">
         <v>275</v>
       </c>
-      <c r="O24" s="405"/>
-      <c r="P24" s="405"/>
-      <c r="Q24" s="405"/>
+      <c r="O24" s="413"/>
+      <c r="P24" s="413"/>
+      <c r="Q24" s="413"/>
       <c r="R24" s="155" t="s">
         <v>6166</v>
       </c>
-      <c r="S24" s="406"/>
+      <c r="S24" s="415"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="S22:S24"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O24"/>
+    <mergeCell ref="P22:P24"/>
+    <mergeCell ref="Q22:Q24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F9:F14"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="G15:G21"/>
+    <mergeCell ref="R18:R21"/>
+    <mergeCell ref="S19:S21"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E17"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="J9:L14"/>
+    <mergeCell ref="N3:N14"/>
+    <mergeCell ref="O9:O18"/>
+    <mergeCell ref="P9:P17"/>
+    <mergeCell ref="R9:R14"/>
+    <mergeCell ref="S9:S14"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O19:P21"/>
+    <mergeCell ref="Q3:Q21"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="K19:K21"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="C3:E8"/>
     <mergeCell ref="I3:L8"/>
@@ -37345,55 +37400,6 @@
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O19:P21"/>
-    <mergeCell ref="Q3:Q21"/>
-    <mergeCell ref="R18:R21"/>
-    <mergeCell ref="S19:S21"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E17"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="J9:L14"/>
-    <mergeCell ref="N3:N14"/>
-    <mergeCell ref="O9:O18"/>
-    <mergeCell ref="P9:P17"/>
-    <mergeCell ref="R9:R14"/>
-    <mergeCell ref="S9:S14"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="C22:E23"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G15:G21"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O24"/>
-    <mergeCell ref="P22:P24"/>
-    <mergeCell ref="Q22:Q24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -81664,7 +81670,7 @@
       <c r="A2" t="s">
         <v>6167</v>
       </c>
-      <c r="B2" s="419" t="s">
+      <c r="B2" s="425" t="s">
         <v>6168</v>
       </c>
     </row>
@@ -81672,7 +81678,7 @@
       <c r="A3" t="s">
         <v>6802</v>
       </c>
-      <c r="B3" s="419"/>
+      <c r="B3" s="425"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -81734,7 +81740,7 @@
       <c r="A11" t="s">
         <v>6183</v>
       </c>
-      <c r="B11" s="419" t="s">
+      <c r="B11" s="425" t="s">
         <v>6185</v>
       </c>
     </row>
@@ -81742,7 +81748,7 @@
       <c r="A12" t="s">
         <v>6184</v>
       </c>
-      <c r="B12" s="419"/>
+      <c r="B12" s="425"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
@@ -81780,7 +81786,7 @@
       <c r="A17" t="s">
         <v>6790</v>
       </c>
-      <c r="B17" s="419" t="s">
+      <c r="B17" s="425" t="s">
         <v>6194</v>
       </c>
     </row>
@@ -81788,7 +81794,7 @@
       <c r="A18" t="s">
         <v>6193</v>
       </c>
-      <c r="B18" s="419"/>
+      <c r="B18" s="425"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
@@ -81818,7 +81824,7 @@
       <c r="A22" t="s">
         <v>6792</v>
       </c>
-      <c r="B22" s="419" t="s">
+      <c r="B22" s="425" t="s">
         <v>6798</v>
       </c>
     </row>
@@ -81826,31 +81832,31 @@
       <c r="A23" t="s">
         <v>6793</v>
       </c>
-      <c r="B23" s="419"/>
+      <c r="B23" s="425"/>
     </row>
     <row r="24" spans="1:2" ht="30">
       <c r="A24" s="313" t="s">
         <v>6794</v>
       </c>
-      <c r="B24" s="419"/>
+      <c r="B24" s="425"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="153" t="s">
         <v>6795</v>
       </c>
-      <c r="B25" s="419"/>
+      <c r="B25" s="425"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>6796</v>
       </c>
-      <c r="B26" s="419"/>
+      <c r="B26" s="425"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>5901</v>
       </c>
-      <c r="B27" s="419"/>
+      <c r="B27" s="425"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">

</xml_diff>